<commit_message>
Components of population change 2011 data prep
</commit_message>
<xml_diff>
--- a/data_demography/04 Components of population change.xlsx
+++ b/data_demography/04 Components of population change.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="161">
   <si>
     <t xml:space="preserve">SPAIN </t>
   </si>
@@ -102,6 +102,9 @@
   </si>
   <si>
     <t xml:space="preserve">Spain 2011 Deaths</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spain Natural increase  2011-12</t>
   </si>
   <si>
     <t xml:space="preserve">Spain 2012 components of population change</t>
@@ -862,8 +865,8 @@
   </sheetPr>
   <dimension ref="A3:C152"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A23" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B34" activeCellId="0" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1141,7 +1144,7 @@
         <v>10</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C34" s="6" t="n">
         <f aca="false">C32-C33</f>
@@ -1167,7 +1170,7 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1186,7 +1189,7 @@
         <v>2</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C39" s="9" t="n">
         <v>46712650</v>
@@ -1197,7 +1200,7 @@
         <v>6</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C40" s="10" t="n">
         <f aca="false">C39-C38</f>
@@ -1209,7 +1212,7 @@
         <v>4</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1217,7 +1220,7 @@
         <v>5</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1225,7 +1228,7 @@
         <v>10</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1243,7 +1246,7 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1251,7 +1254,7 @@
         <v>1</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C47" s="9" t="n">
         <v>46712650</v>
@@ -1262,7 +1265,7 @@
         <v>2</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C48" s="9" t="n">
         <v>46495744</v>
@@ -1273,7 +1276,7 @@
         <v>6</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C49" s="10" t="n">
         <f aca="false">C48-C47</f>
@@ -1285,7 +1288,7 @@
         <v>4</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1293,7 +1296,7 @@
         <v>5</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1301,7 +1304,7 @@
         <v>10</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1319,7 +1322,7 @@
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1327,7 +1330,7 @@
         <v>1</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C56" s="9" t="n">
         <v>46495744</v>
@@ -1338,7 +1341,7 @@
         <v>2</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C57" s="9" t="n">
         <v>46425722</v>
@@ -1349,7 +1352,7 @@
         <v>6</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C58" s="10" t="n">
         <f aca="false">C57-C56</f>
@@ -1361,7 +1364,7 @@
         <v>4</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1369,7 +1372,7 @@
         <v>5</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1377,7 +1380,7 @@
         <v>10</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1395,7 +1398,7 @@
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B64" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1403,7 +1406,7 @@
         <v>1</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C65" s="9" t="n">
         <v>46425722</v>
@@ -1414,7 +1417,7 @@
         <v>2</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C66" s="9" t="n">
         <v>46418884</v>
@@ -1425,7 +1428,7 @@
         <v>6</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C67" s="10" t="n">
         <f aca="false">C66-C65</f>
@@ -1437,7 +1440,7 @@
         <v>4</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1445,7 +1448,7 @@
         <v>5</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1453,7 +1456,7 @@
         <v>10</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1471,7 +1474,7 @@
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B73" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1479,7 +1482,7 @@
         <v>1</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C74" s="9" t="n">
         <v>46418884</v>
@@ -1490,7 +1493,7 @@
         <v>2</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C75" s="9" t="n">
         <v>46497393</v>
@@ -1501,7 +1504,7 @@
         <v>6</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C76" s="10" t="n">
         <f aca="false">C75-C74</f>
@@ -1513,7 +1516,7 @@
         <v>4</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1521,7 +1524,7 @@
         <v>5</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1529,7 +1532,7 @@
         <v>10</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1547,7 +1550,7 @@
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B82" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1555,7 +1558,7 @@
         <v>1</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C83" s="9" t="n">
         <v>46497393</v>
@@ -1566,7 +1569,7 @@
         <v>2</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C84" s="9" t="n">
         <v>46645070</v>
@@ -1577,7 +1580,7 @@
         <v>6</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C85" s="10" t="n">
         <f aca="false">C84-C83</f>
@@ -1589,7 +1592,7 @@
         <v>4</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1597,7 +1600,7 @@
         <v>5</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1605,7 +1608,7 @@
         <v>10</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1623,7 +1626,7 @@
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B91" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1631,7 +1634,7 @@
         <v>1</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C92" s="9" t="n">
         <v>46645070</v>
@@ -1642,7 +1645,7 @@
         <v>2</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C93" s="9" t="n">
         <v>46918951</v>
@@ -1653,7 +1656,7 @@
         <v>6</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C94" s="10" t="n">
         <f aca="false">C93-C92</f>
@@ -1665,7 +1668,7 @@
         <v>4</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1673,7 +1676,7 @@
         <v>5</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1681,7 +1684,7 @@
         <v>10</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1699,7 +1702,7 @@
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B100" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1707,7 +1710,7 @@
         <v>1</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C101" s="9" t="n">
         <v>46918951</v>
@@ -1718,7 +1721,7 @@
         <v>2</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C102" s="9" t="n">
         <v>47318050</v>
@@ -1729,7 +1732,7 @@
         <v>6</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C103" s="10" t="n">
         <f aca="false">C102-C101</f>
@@ -1741,7 +1744,7 @@
         <v>4</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1749,7 +1752,7 @@
         <v>5</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1757,7 +1760,7 @@
         <v>10</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1775,7 +1778,7 @@
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B109" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1783,7 +1786,7 @@
         <v>1</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C110" s="9" t="n">
         <v>47318050</v>
@@ -1794,7 +1797,7 @@
         <v>2</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C111" s="9" t="n">
         <v>47400798</v>
@@ -1805,7 +1808,7 @@
         <v>6</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C112" s="10" t="n">
         <f aca="false">C111-C110</f>
@@ -1817,7 +1820,7 @@
         <v>4</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1825,7 +1828,7 @@
         <v>5</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1833,7 +1836,7 @@
         <v>10</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1851,7 +1854,7 @@
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B118" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1859,7 +1862,7 @@
         <v>1</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C119" s="9" t="n">
         <v>47400798</v>
@@ -1870,7 +1873,7 @@
         <v>2</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C120" s="9" t="n">
         <v>47486727</v>
@@ -1881,7 +1884,7 @@
         <v>6</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C121" s="10" t="n">
         <f aca="false">C120-C119</f>
@@ -1893,7 +1896,7 @@
         <v>4</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1901,7 +1904,7 @@
         <v>5</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1909,7 +1912,7 @@
         <v>10</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1927,7 +1930,7 @@
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B127" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1935,7 +1938,7 @@
         <v>1</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C128" s="9" t="n">
         <v>47486727</v>
@@ -1946,7 +1949,7 @@
         <v>2</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C129" s="9" t="n">
         <v>48085361</v>
@@ -1957,7 +1960,7 @@
         <v>6</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C130" s="10" t="n">
         <f aca="false">C129-C128</f>
@@ -1969,7 +1972,7 @@
         <v>4</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1977,7 +1980,7 @@
         <v>5</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1985,7 +1988,7 @@
         <v>10</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2003,7 +2006,7 @@
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B136" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2011,7 +2014,7 @@
         <v>1</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C137" s="9" t="n">
         <v>48085361</v>
@@ -2022,7 +2025,7 @@
         <v>2</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C138" s="9" t="n">
         <v>48619695</v>
@@ -2033,7 +2036,7 @@
         <v>6</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C139" s="10" t="n">
         <f aca="false">C138-C137</f>
@@ -2045,7 +2048,7 @@
         <v>4</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2053,7 +2056,7 @@
         <v>5</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2061,7 +2064,7 @@
         <v>10</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2079,7 +2082,7 @@
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B145" s="3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2087,7 +2090,7 @@
         <v>1</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C146" s="9" t="n">
         <v>48619695</v>
@@ -2098,7 +2101,7 @@
         <v>2</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2106,7 +2109,7 @@
         <v>6</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2114,7 +2117,7 @@
         <v>4</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2122,7 +2125,7 @@
         <v>5</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2130,7 +2133,7 @@
         <v>10</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2171,7 +2174,7 @@
   <sheetData>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="12" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
@@ -2186,7 +2189,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2194,21 +2197,21 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="13" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="13" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B6" s="9" t="n">
         <v>42547454</v>
@@ -2218,7 +2221,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="13" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B7" s="9" t="n">
         <v>43296335</v>
@@ -2234,7 +2237,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="13" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B8" s="9" t="n">
         <v>44009969</v>
@@ -2250,7 +2253,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="13" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B9" s="9" t="n">
         <v>44784659</v>
@@ -2266,7 +2269,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="13" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B10" s="9" t="n">
         <v>45668938</v>
@@ -2283,7 +2286,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="13" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B11" s="9" t="n">
         <v>46239271</v>
@@ -2299,7 +2302,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="13" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B12" s="9" t="n">
         <v>46486621</v>
@@ -2315,7 +2318,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="13" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B13" s="9" t="n">
         <v>46667175</v>
@@ -2331,7 +2334,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="13" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B14" s="9" t="n">
         <v>46818216</v>
@@ -2347,7 +2350,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="13" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B15" s="9" t="n">
         <v>46712650</v>
@@ -2363,7 +2366,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="13" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B16" s="9" t="n">
         <v>46495744</v>
@@ -2379,7 +2382,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="13" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B17" s="9" t="n">
         <v>46425722</v>
@@ -2395,7 +2398,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="13" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B18" s="9" t="n">
         <v>46418884</v>
@@ -2411,7 +2414,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="13" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B19" s="9" t="n">
         <v>46497393</v>
@@ -2427,7 +2430,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="13" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B20" s="9" t="n">
         <v>46645070</v>
@@ -2443,7 +2446,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="13" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B21" s="9" t="n">
         <v>46918951</v>
@@ -2459,7 +2462,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="13" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B22" s="9" t="n">
         <v>47318050</v>
@@ -2475,7 +2478,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="13" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B23" s="9" t="n">
         <v>47400798</v>
@@ -2491,7 +2494,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="13" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B24" s="9" t="n">
         <v>47486727</v>
@@ -2507,7 +2510,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="13" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B25" s="9" t="n">
         <v>48085361</v>
@@ -2523,7 +2526,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="13" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B26" s="9" t="n">
         <v>48619695</v>
@@ -2567,26 +2570,26 @@
   <sheetData>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2841,28 +2844,28 @@
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2947,7 +2950,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="7" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -2980,104 +2983,104 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="7" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="54.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="18" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="19" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="79.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="19" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="19" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B10" s="19" t="n">
         <v>345.238</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="19" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B11" s="19" t="n">
         <v>425.363</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="19" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B12" s="19" t="n">
         <v>80.125</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="19" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B13" s="19" t="n">
         <v>55.706</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="19" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B14" s="19" t="n">
         <v>25.968</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="19" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B15" s="19" t="n">
         <v>29.738</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="19" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B16" s="19" t="n">
         <v>50.387</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
start populating 2023 GT table
</commit_message>
<xml_diff>
--- a/data_demography/04 Components of population change.xlsx
+++ b/data_demography/04 Components of population change.xlsx
@@ -865,8 +865,8 @@
   </sheetPr>
   <dimension ref="A3:C152"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A23" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B34" activeCellId="0" sqref="B34"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A133" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C144" activeCellId="0" sqref="C144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2050,6 +2050,9 @@
       <c r="B140" s="1" t="s">
         <v>95</v>
       </c>
+      <c r="C140" s="11" t="n">
+        <v>320656</v>
+      </c>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="4" t="n">
@@ -2058,6 +2061,9 @@
       <c r="B141" s="1" t="s">
         <v>96</v>
       </c>
+      <c r="C141" s="11" t="n">
+        <v>436124</v>
+      </c>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="4" t="s">
@@ -2066,6 +2072,10 @@
       <c r="B142" s="1" t="s">
         <v>97</v>
       </c>
+      <c r="C142" s="6" t="n">
+        <f aca="false">C140-C141</f>
+        <v>-115468</v>
+      </c>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="4" t="s">
@@ -2073,6 +2083,10 @@
       </c>
       <c r="B143" s="7" t="s">
         <v>13</v>
+      </c>
+      <c r="C143" s="8" t="n">
+        <f aca="false">C139-C142</f>
+        <v>649802</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2563,7 +2577,7 @@
   <dimension ref="A3:D20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G30" activeCellId="0" sqref="G30"/>
+      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
changed labels Excel input file first two rows
</commit_message>
<xml_diff>
--- a/data_demography/04 Components of population change.xlsx
+++ b/data_demography/04 Components of population change.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="162">
   <si>
     <t xml:space="preserve">SPAIN </t>
   </si>
@@ -308,7 +308,10 @@
     <t xml:space="preserve">Spain 2023 components of population change</t>
   </si>
   <si>
-    <t xml:space="preserve">Spain 2024 total population</t>
+    <t xml:space="preserve">Spain resident population as of January 1st  2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spain resident population as of January 1st  2024</t>
   </si>
   <si>
     <t xml:space="preserve">Spain population change 2023-24 </t>
@@ -326,7 +329,7 @@
     <t xml:space="preserve">Spain 2024 components of population change</t>
   </si>
   <si>
-    <t xml:space="preserve">Spain 2025 total population</t>
+    <t xml:space="preserve">Spain resident population as of January 1st  2025</t>
   </si>
   <si>
     <t xml:space="preserve">Spain population change 2024-25</t>
@@ -866,7 +869,7 @@
   <dimension ref="A3:C152"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A133" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C144" activeCellId="0" sqref="C144"/>
+      <selection pane="topLeft" activeCell="E142" activeCellId="0" sqref="E142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2014,7 +2017,7 @@
         <v>1</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="C137" s="9" t="n">
         <v>48085361</v>
@@ -2025,7 +2028,7 @@
         <v>2</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C138" s="9" t="n">
         <v>48619695</v>
@@ -2036,7 +2039,7 @@
         <v>6</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C139" s="10" t="n">
         <f aca="false">C138-C137</f>
@@ -2048,7 +2051,7 @@
         <v>4</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C140" s="11" t="n">
         <v>320656</v>
@@ -2059,7 +2062,7 @@
         <v>5</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C141" s="11" t="n">
         <v>436124</v>
@@ -2070,7 +2073,7 @@
         <v>10</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C142" s="6" t="n">
         <f aca="false">C140-C141</f>
@@ -2096,7 +2099,7 @@
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B145" s="3" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2104,7 +2107,7 @@
         <v>1</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C146" s="9" t="n">
         <v>48619695</v>
@@ -2115,7 +2118,7 @@
         <v>2</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2123,7 +2126,7 @@
         <v>6</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2131,7 +2134,7 @@
         <v>4</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2139,7 +2142,7 @@
         <v>5</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2147,7 +2150,7 @@
         <v>10</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2188,7 +2191,7 @@
   <sheetData>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="12" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
@@ -2203,7 +2206,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2211,21 +2214,21 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="13" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="13" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B6" s="9" t="n">
         <v>42547454</v>
@@ -2235,7 +2238,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="13" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B7" s="9" t="n">
         <v>43296335</v>
@@ -2251,7 +2254,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="13" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B8" s="9" t="n">
         <v>44009969</v>
@@ -2267,7 +2270,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="13" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B9" s="9" t="n">
         <v>44784659</v>
@@ -2283,7 +2286,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="13" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B10" s="9" t="n">
         <v>45668938</v>
@@ -2300,7 +2303,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="13" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B11" s="9" t="n">
         <v>46239271</v>
@@ -2316,7 +2319,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="13" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B12" s="9" t="n">
         <v>46486621</v>
@@ -2332,7 +2335,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="13" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B13" s="9" t="n">
         <v>46667175</v>
@@ -2348,7 +2351,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="13" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B14" s="9" t="n">
         <v>46818216</v>
@@ -2364,7 +2367,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="13" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B15" s="9" t="n">
         <v>46712650</v>
@@ -2380,7 +2383,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="13" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B16" s="9" t="n">
         <v>46495744</v>
@@ -2396,7 +2399,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="13" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B17" s="9" t="n">
         <v>46425722</v>
@@ -2412,7 +2415,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="13" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B18" s="9" t="n">
         <v>46418884</v>
@@ -2428,7 +2431,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="13" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B19" s="9" t="n">
         <v>46497393</v>
@@ -2444,7 +2447,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="13" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B20" s="9" t="n">
         <v>46645070</v>
@@ -2460,7 +2463,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="13" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B21" s="9" t="n">
         <v>46918951</v>
@@ -2476,7 +2479,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="13" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B22" s="9" t="n">
         <v>47318050</v>
@@ -2492,7 +2495,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="13" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B23" s="9" t="n">
         <v>47400798</v>
@@ -2508,7 +2511,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="13" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B24" s="9" t="n">
         <v>47486727</v>
@@ -2524,7 +2527,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="13" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B25" s="9" t="n">
         <v>48085361</v>
@@ -2540,7 +2543,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="13" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B26" s="9" t="n">
         <v>48619695</v>
@@ -2584,26 +2587,26 @@
   <sheetData>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2858,28 +2861,28 @@
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2964,7 +2967,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="7" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -2997,104 +3000,104 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="7" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="54.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="18" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="19" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="79.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="19" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="19" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B10" s="19" t="n">
         <v>345.238</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="19" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B11" s="19" t="n">
         <v>425.363</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="19" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B12" s="19" t="n">
         <v>80.125</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="19" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B13" s="19" t="n">
         <v>55.706</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="19" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B14" s="19" t="n">
         <v>25.968</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="19" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B15" s="19" t="n">
         <v>29.738</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="19" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B16" s="19" t="n">
         <v>50.387</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating deahts and births excel file
</commit_message>
<xml_diff>
--- a/data_demography/04 Components of population change.xlsx
+++ b/data_demography/04 Components of population change.xlsx
@@ -8,11 +8,11 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="SPAIN_Components_pop_change" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="INE Total Population SPAIN" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="INE National Increase SPAIN" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="INE Net External Migration" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="Template comp pop change" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="SPAIN_Components_pop_change" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="INE Total Population SPAIN" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="INE National Increase SPAIN" sheetId="3" state="visible" r:id="rId5"/>
+    <sheet name="INE Net External Migration" sheetId="4" state="visible" r:id="rId6"/>
+    <sheet name="Template comp pop change" sheetId="5" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" name="maincontent" vbProcedure="false">'Template comp pop change'!$A$4</definedName>
@@ -860,6 +860,112 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -868,11 +974,11 @@
   </sheetPr>
   <dimension ref="A3:C152"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A133" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E142" activeCellId="0" sqref="E142"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A115" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C132" activeCellId="0" sqref="C132"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="53.3"/>
@@ -1217,6 +1323,9 @@
       <c r="B41" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="C41" s="11" t="n">
+        <v>454648</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="4" t="n">
@@ -1225,6 +1334,9 @@
       <c r="B42" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="C42" s="11" t="n">
+        <v>402950</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="4" t="s">
@@ -1293,6 +1405,9 @@
       <c r="B50" s="1" t="s">
         <v>35</v>
       </c>
+      <c r="C50" s="11" t="n">
+        <v>425715</v>
+      </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="4" t="n">
@@ -1301,6 +1416,9 @@
       <c r="B51" s="1" t="s">
         <v>36</v>
       </c>
+      <c r="C51" s="11" t="n">
+        <v>390419</v>
+      </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="4" t="s">
@@ -1369,6 +1487,9 @@
       <c r="B59" s="1" t="s">
         <v>41</v>
       </c>
+      <c r="C59" s="11" t="n">
+        <v>427595</v>
+      </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="4" t="n">
@@ -1377,6 +1498,9 @@
       <c r="B60" s="1" t="s">
         <v>42</v>
       </c>
+      <c r="C60" s="11" t="n">
+        <v>395830</v>
+      </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="4" t="s">
@@ -1445,6 +1569,9 @@
       <c r="B68" s="1" t="s">
         <v>47</v>
       </c>
+      <c r="C68" s="11" t="n">
+        <v>420290</v>
+      </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="4" t="n">
@@ -1453,6 +1580,9 @@
       <c r="B69" s="1" t="s">
         <v>48</v>
       </c>
+      <c r="C69" s="11" t="n">
+        <v>422568</v>
+      </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="4" t="s">
@@ -1521,6 +1651,9 @@
       <c r="B77" s="1" t="s">
         <v>53</v>
       </c>
+      <c r="C77" s="11" t="n">
+        <v>410583</v>
+      </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="4" t="n">
@@ -1529,6 +1662,9 @@
       <c r="B78" s="1" t="s">
         <v>54</v>
       </c>
+      <c r="C78" s="11" t="n">
+        <v>410611</v>
+      </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="4" t="s">
@@ -1597,6 +1733,9 @@
       <c r="B86" s="1" t="s">
         <v>59</v>
       </c>
+      <c r="C86" s="11" t="n">
+        <v>393181</v>
+      </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="4" t="n">
@@ -1605,6 +1744,9 @@
       <c r="B87" s="1" t="s">
         <v>60</v>
       </c>
+      <c r="C87" s="11" t="n">
+        <v>424523</v>
+      </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="4" t="s">
@@ -1673,6 +1815,9 @@
       <c r="B95" s="1" t="s">
         <v>65</v>
       </c>
+      <c r="C95" s="11" t="n">
+        <v>372777</v>
+      </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="4" t="n">
@@ -1681,6 +1826,9 @@
       <c r="B96" s="1" t="s">
         <v>66</v>
       </c>
+      <c r="C96" s="11" t="n">
+        <v>427721</v>
+      </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="4" t="s">
@@ -1749,6 +1897,9 @@
       <c r="B104" s="1" t="s">
         <v>71</v>
       </c>
+      <c r="C104" s="11" t="n">
+        <v>360617</v>
+      </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="4" t="n">
@@ -1757,6 +1908,9 @@
       <c r="B105" s="1" t="s">
         <v>72</v>
       </c>
+      <c r="C105" s="11" t="n">
+        <v>418703</v>
+      </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="4" t="s">
@@ -1825,6 +1979,9 @@
       <c r="B113" s="1" t="s">
         <v>77</v>
       </c>
+      <c r="C113" s="11" t="n">
+        <v>341315</v>
+      </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="4" t="n">
@@ -1833,6 +1990,9 @@
       <c r="B114" s="1" t="s">
         <v>78</v>
       </c>
+      <c r="C114" s="11" t="n">
+        <v>493776</v>
+      </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="4" t="s">
@@ -1901,6 +2061,9 @@
       <c r="B122" s="1" t="s">
         <v>83</v>
       </c>
+      <c r="C122" s="11" t="n">
+        <v>337380</v>
+      </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="4" t="n">
@@ -1909,6 +2072,9 @@
       <c r="B123" s="1" t="s">
         <v>84</v>
       </c>
+      <c r="C123" s="11" t="n">
+        <v>450744</v>
+      </c>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="4" t="s">
@@ -1977,6 +2143,9 @@
       <c r="B131" s="1" t="s">
         <v>89</v>
       </c>
+      <c r="C131" s="11" t="n">
+        <v>329251</v>
+      </c>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="4" t="n">
@@ -1984,6 +2153,9 @@
       </c>
       <c r="B132" s="1" t="s">
         <v>90</v>
+      </c>
+      <c r="C132" s="11" t="n">
+        <v>464417</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2166,8 +2338,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -2180,11 +2352,11 @@
   </sheetPr>
   <dimension ref="A2:K26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18.07"/>
   </cols>
@@ -2565,8 +2737,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -2579,11 +2751,11 @@
   </sheetPr>
   <dimension ref="A3:D20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
@@ -2839,8 +3011,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -2853,11 +3025,11 @@
   </sheetPr>
   <dimension ref="A2:B20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I30" activeCellId="0" sqref="I30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5234375" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
@@ -2975,8 +3147,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -2988,11 +3160,11 @@
   </sheetPr>
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C29" activeCellId="0" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="7" width="42.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="7" width="24.67"/>
@@ -3008,7 +3180,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="19" t="s">
         <v>146</v>
       </c>
@@ -3105,8 +3277,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
computed residual migration each individual year
</commit_message>
<xml_diff>
--- a/data_demography/04 Components of population change.xlsx
+++ b/data_demography/04 Components of population change.xlsx
@@ -975,7 +975,7 @@
   <dimension ref="A3:C152"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A115" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C142" activeCellId="0" sqref="C142"/>
+      <selection pane="topLeft" activeCell="C143" activeCellId="0" sqref="C143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1357,6 +1357,10 @@
       <c r="B44" s="7" t="s">
         <v>13</v>
       </c>
+      <c r="C44" s="8" t="n">
+        <f aca="false">C40-C43</f>
+        <v>-157264</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="3" t="n">
@@ -1443,6 +1447,10 @@
       <c r="B53" s="7" t="s">
         <v>13</v>
       </c>
+      <c r="C53" s="8" t="n">
+        <f aca="false">C49-C52</f>
+        <v>-252202</v>
+      </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="3" t="n">
@@ -1529,6 +1537,10 @@
       <c r="B62" s="7" t="s">
         <v>13</v>
       </c>
+      <c r="C62" s="8" t="n">
+        <f aca="false">C58-C61</f>
+        <v>-101787</v>
+      </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="3" t="n">
@@ -1615,6 +1627,10 @@
       <c r="B71" s="7" t="s">
         <v>13</v>
       </c>
+      <c r="C71" s="8" t="n">
+        <f aca="false">C67-C70</f>
+        <v>-4560</v>
+      </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="3" t="n">
@@ -1701,6 +1717,10 @@
       <c r="B80" s="7" t="s">
         <v>13</v>
       </c>
+      <c r="C80" s="8" t="n">
+        <f aca="false">C76-C79</f>
+        <v>78537</v>
+      </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="3" t="n">
@@ -1787,6 +1807,10 @@
       <c r="B89" s="7" t="s">
         <v>13</v>
       </c>
+      <c r="C89" s="8" t="n">
+        <f aca="false">C85-C88</f>
+        <v>179019</v>
+      </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="3" t="n">
@@ -1873,6 +1897,10 @@
       <c r="B98" s="7" t="s">
         <v>13</v>
       </c>
+      <c r="C98" s="8" t="n">
+        <f aca="false">C94-C97</f>
+        <v>328825</v>
+      </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="3" t="n">
@@ -1959,6 +1987,10 @@
       <c r="B107" s="7" t="s">
         <v>13</v>
       </c>
+      <c r="C107" s="8" t="n">
+        <f aca="false">C103-C106</f>
+        <v>457185</v>
+      </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="3" t="n">
@@ -2045,6 +2077,10 @@
       <c r="B116" s="7" t="s">
         <v>13</v>
       </c>
+      <c r="C116" s="8" t="n">
+        <f aca="false">C112-C115</f>
+        <v>235209</v>
+      </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="3" t="n">
@@ -2131,6 +2167,10 @@
       <c r="B125" s="7" t="s">
         <v>13</v>
       </c>
+      <c r="C125" s="8" t="n">
+        <f aca="false">C121-C124</f>
+        <v>199293</v>
+      </c>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="3" t="n">
@@ -2216,6 +2256,10 @@
       </c>
       <c r="B134" s="7" t="s">
         <v>13</v>
+      </c>
+      <c r="C134" s="8" t="n">
+        <f aca="false">C130-C133</f>
+        <v>733800</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2397,7 +2441,7 @@
   <dimension ref="A2:K26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B26" activeCellId="1" sqref="C142 B26"/>
+      <selection pane="topLeft" activeCell="B26" activeCellId="1" sqref="C143 B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2796,7 +2840,7 @@
   <dimension ref="A3:D20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C19" activeCellId="1" sqref="C142 C19"/>
+      <selection pane="topLeft" activeCell="C19" activeCellId="1" sqref="C143 C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3070,7 +3114,7 @@
   <dimension ref="A2:B20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I30" activeCellId="1" sqref="C142 I30"/>
+      <selection pane="topLeft" activeCell="I30" activeCellId="1" sqref="C143 I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5234375" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3205,7 +3249,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C29" activeCellId="1" sqref="C142 C29"/>
+      <selection pane="topLeft" activeCell="C29" activeCellId="1" sqref="C143 C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>